<commit_message>
Change Java Version 17 -> 8, add charts
</commit_message>
<xml_diff>
--- a/L2/measurements/wykresy.xlsx
+++ b/L2/measurements/wykresy.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="37" documentId="8_{04DB1D78-4E98-4EC5-A9E8-7C82D1C0C81C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D305340-D6D9-49CE-B641-5F3794B188FA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="746" xr2:uid="{C0DDF5A4-2B5D-41D6-A5A5-87E6897D9B4D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="746" xr2:uid="{C0DDF5A4-2B5D-41D6-A5A5-87E6897D9B4D}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="9" r:id="rId1"/>
@@ -31851,10 +31851,10 @@
     <tableColumn id="1" xr3:uid="{E48162D0-F690-40DE-9815-38EA828519D9}" uniqueName="1" name="n" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{4391557E-0953-4D01-982E-B4FC30240933}" uniqueName="2" name="c" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{D9E39EA7-E0AF-463D-8B9E-2592BA9F7A6D}" uniqueName="3" name="s" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{18BA3F71-576B-4F4D-A4B0-FFFCCC10DE30}" uniqueName="4" name="c/n" queryTableFieldId="4" dataDxfId="21">
+    <tableColumn id="4" xr3:uid="{18BA3F71-576B-4F4D-A4B0-FFFCCC10DE30}" uniqueName="4" name="c/n" queryTableFieldId="4" dataDxfId="23">
       <calculatedColumnFormula>MergeSort1009[[#This Row],[c]]/MergeSort1009[[#This Row],[n]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2F2659F1-0542-4AC5-B7D7-5269BC04E1EE}" uniqueName="7" name="s/n" queryTableFieldId="5" dataDxfId="16">
+    <tableColumn id="7" xr3:uid="{2F2659F1-0542-4AC5-B7D7-5269BC04E1EE}" uniqueName="7" name="s/n" queryTableFieldId="5" dataDxfId="22">
       <calculatedColumnFormula>MergeSort1009[[#This Row],[s]]/MergeSort1009[[#This Row],[n]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -31923,10 +31923,10 @@
     <tableColumn id="1" xr3:uid="{1399EDD3-1764-486B-8897-55BB5F8AE10F}" uniqueName="1" name="n" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{7D682038-8B25-41DE-8284-6064EFE1D3C4}" uniqueName="2" name="c" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{A382F725-C424-41DE-B015-9C4C15AE02E8}" uniqueName="3" name="s" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{1EEF4306-6C05-4644-AA92-5986A0BBBE50}" uniqueName="4" name="c/n" queryTableFieldId="4" dataDxfId="20">
+    <tableColumn id="4" xr3:uid="{1EEF4306-6C05-4644-AA92-5986A0BBBE50}" uniqueName="4" name="c/n" queryTableFieldId="4" dataDxfId="21">
       <calculatedColumnFormula>InsertionSort10010[[#This Row],[c]]/InsertionSort10010[[#This Row],[n]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{0FF3B983-A5E5-484D-AF06-3D2862C76F1E}" uniqueName="5" name="s/n" queryTableFieldId="5" dataDxfId="19">
+    <tableColumn id="5" xr3:uid="{0FF3B983-A5E5-484D-AF06-3D2862C76F1E}" uniqueName="5" name="s/n" queryTableFieldId="5" dataDxfId="20">
       <calculatedColumnFormula>InsertionSort10010[[#This Row],[s]]/InsertionSort10010[[#This Row],[n]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -31941,10 +31941,10 @@
     <tableColumn id="1" xr3:uid="{F04C64DD-E890-4701-8E26-08371B578E3E}" uniqueName="1" name="n" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{458415B9-5239-48B3-BDBD-5D014C3839C9}" uniqueName="2" name="c" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{F3CC5512-8DE7-47D0-808A-138A5B71D460}" uniqueName="3" name="s" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{ADA9E380-F42F-40C7-8CD4-17717B771CDC}" uniqueName="4" name="c/n" queryTableFieldId="4" dataDxfId="18">
+    <tableColumn id="4" xr3:uid="{ADA9E380-F42F-40C7-8CD4-17717B771CDC}" uniqueName="4" name="c/n" queryTableFieldId="4" dataDxfId="19">
       <calculatedColumnFormula>QuickSort10012[[#This Row],[c]]/QuickSort10012[[#This Row],[n]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C58BA89C-656D-4B0D-9C1F-44F6A1BCA5AD}" uniqueName="5" name="s/n" queryTableFieldId="5" dataDxfId="17">
+    <tableColumn id="5" xr3:uid="{C58BA89C-656D-4B0D-9C1F-44F6A1BCA5AD}" uniqueName="5" name="s/n" queryTableFieldId="5" dataDxfId="18">
       <calculatedColumnFormula>QuickSort10012[[#This Row],[s]]/QuickSort10012[[#This Row],[n]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -31959,10 +31959,10 @@
     <tableColumn id="1" xr3:uid="{8CCF0240-E1ED-462B-AD66-C417A21A2AA3}" uniqueName="1" name="n" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{52B81960-F0E7-4B58-8A25-F843F44CC928}" uniqueName="2" name="c" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{D34DDD4F-37D9-4C39-8B04-E99A9F8408C6}" uniqueName="3" name="s" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{7C0790BF-44A1-42B5-AD44-72FE07361437}" uniqueName="4" name="c/n" queryTableFieldId="4" dataDxfId="11">
+    <tableColumn id="4" xr3:uid="{7C0790BF-44A1-42B5-AD44-72FE07361437}" uniqueName="4" name="c/n" queryTableFieldId="4" dataDxfId="17">
       <calculatedColumnFormula>DualPivotQuickSort1001819[[#This Row],[c]]/DualPivotQuickSort1001819[[#This Row],[n]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{09C68719-6B09-41E0-9A17-AA1E1A17444D}" uniqueName="5" name="s/n" queryTableFieldId="5" dataDxfId="10">
+    <tableColumn id="5" xr3:uid="{09C68719-6B09-41E0-9A17-AA1E1A17444D}" uniqueName="5" name="s/n" queryTableFieldId="5" dataDxfId="16">
       <calculatedColumnFormula>DualPivotQuickSort1001819[[#This Row],[s]]/DualPivotQuickSort1001819[[#This Row],[n]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -31977,10 +31977,10 @@
     <tableColumn id="1" xr3:uid="{1F663BC3-3C55-4F23-811B-CDC50E7FF3CA}" uniqueName="1" name="n" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{4ED98A11-6EDD-4AEE-8FC8-CCBC31175FE2}" uniqueName="2" name="c" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{50FCD642-BD9F-46B0-9BDE-319E45C182B8}" uniqueName="3" name="s" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{22EC6A42-F2AD-47BB-A3E1-B582C40DFCB0}" uniqueName="4" name="c/n" queryTableFieldId="4" dataDxfId="13">
+    <tableColumn id="4" xr3:uid="{22EC6A42-F2AD-47BB-A3E1-B582C40DFCB0}" uniqueName="4" name="c/n" queryTableFieldId="4" dataDxfId="15">
       <calculatedColumnFormula>DualPivotQuickSort10018[[#This Row],[c]]/DualPivotQuickSort10018[[#This Row],[n]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{2861435C-65E3-46A0-ACAA-11ED308AC204}" uniqueName="5" name="s/n" queryTableFieldId="5" dataDxfId="12">
+    <tableColumn id="5" xr3:uid="{2861435C-65E3-46A0-ACAA-11ED308AC204}" uniqueName="5" name="s/n" queryTableFieldId="5" dataDxfId="14">
       <calculatedColumnFormula>DualPivotQuickSort10018[[#This Row],[s]]/DualPivotQuickSort10018[[#This Row],[n]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -31995,10 +31995,10 @@
     <tableColumn id="1" xr3:uid="{92BDF992-D3F4-4C77-9B35-50EC30BF06DB}" uniqueName="1" name="n" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{A146671E-4267-4477-B914-ECC8A34E5AAD}" uniqueName="2" name="c" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{1A76CB00-3FB6-4DB6-8F03-EFDC9D76C1AC}" uniqueName="3" name="s" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{22B7E81A-7686-450B-A15D-640AB488D72B}" uniqueName="4" name="c/n" queryTableFieldId="4" dataDxfId="15">
+    <tableColumn id="4" xr3:uid="{22B7E81A-7686-450B-A15D-640AB488D72B}" uniqueName="4" name="c/n" queryTableFieldId="4" dataDxfId="13">
       <calculatedColumnFormula>QuickSort10014[[#This Row],[c]]/QuickSort10014[[#This Row],[n]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{3A39EF91-F4FF-428A-ABA2-00E8897E0DCF}" uniqueName="5" name="s/n" queryTableFieldId="5" dataDxfId="14">
+    <tableColumn id="5" xr3:uid="{3A39EF91-F4FF-428A-ABA2-00E8897E0DCF}" uniqueName="5" name="s/n" queryTableFieldId="5" dataDxfId="12">
       <calculatedColumnFormula>QuickSort10014[[#This Row],[s]]/QuickSort10014[[#This Row],[n]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -32013,10 +32013,10 @@
     <tableColumn id="1" xr3:uid="{57636ACE-33CF-4B5F-B53D-133E2E6757F1}" uniqueName="1" name="n" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{906C8EDA-29D5-4996-853E-7C4DA9EF4D65}" uniqueName="2" name="c" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{8E54BE3F-81C5-4BDB-A803-BB57B367D07B}" uniqueName="3" name="s" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{A1EBA102-FDE6-4B78-B0D2-70A81E955418}" uniqueName="4" name="c/n" queryTableFieldId="4" dataDxfId="22">
+    <tableColumn id="4" xr3:uid="{A1EBA102-FDE6-4B78-B0D2-70A81E955418}" uniqueName="4" name="c/n" queryTableFieldId="4" dataDxfId="11">
       <calculatedColumnFormula>InsertionSort100[[#This Row],[c]]/InsertionSort100[[#This Row],[n]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{89AA8A89-D8A3-4E93-B4AE-0BAD1C24D75F}" uniqueName="5" name="s/n" queryTableFieldId="5" dataDxfId="23">
+    <tableColumn id="5" xr3:uid="{89AA8A89-D8A3-4E93-B4AE-0BAD1C24D75F}" uniqueName="5" name="s/n" queryTableFieldId="5" dataDxfId="10">
       <calculatedColumnFormula>InsertionSort100[[#This Row],[s]]/InsertionSort100[[#This Row],[n]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -32031,10 +32031,10 @@
     <tableColumn id="1" xr3:uid="{9025CA1F-0CBF-4310-93E8-AE6836E4162D}" uniqueName="1" name="n" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{EBE32FC8-1C65-47B1-AFBB-C9BCAA005A8A}" uniqueName="2" name="c" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{83EA4688-74C5-4A4B-8D19-FC956CE746E4}" uniqueName="3" name="s" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{F8173A33-21F1-47D2-9EB4-A17F545A537C}" uniqueName="4" name="c/n" queryTableFieldId="4" dataDxfId="7">
+    <tableColumn id="4" xr3:uid="{F8173A33-21F1-47D2-9EB4-A17F545A537C}" uniqueName="4" name="c/n" queryTableFieldId="4" dataDxfId="9">
       <calculatedColumnFormula>InsertionSort1002022[[#This Row],[c]]/InsertionSort1002022[[#This Row],[n]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B0EE38F7-4253-464B-BFC2-3416B192310F}" uniqueName="5" name="s/n" queryTableFieldId="5" dataDxfId="6">
+    <tableColumn id="5" xr3:uid="{B0EE38F7-4253-464B-BFC2-3416B192310F}" uniqueName="5" name="s/n" queryTableFieldId="5" dataDxfId="8">
       <calculatedColumnFormula>InsertionSort1002022[[#This Row],[s]]/InsertionSort1002022[[#This Row],[n]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -32049,10 +32049,10 @@
     <tableColumn id="1" xr3:uid="{ED896C74-BAAC-4038-80ED-D5BFCEE4AFC8}" uniqueName="1" name="n" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{5361FC46-27F3-47C3-B157-77A935F53157}" uniqueName="2" name="c" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{FDBB2CE9-02EF-4871-A8D5-9F9A4DAC46FE}" uniqueName="3" name="s" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{BB74769A-FCB4-4F87-8BF2-9BC1510C5FCB}" uniqueName="4" name="c/n" queryTableFieldId="4" dataDxfId="9">
+    <tableColumn id="4" xr3:uid="{BB74769A-FCB4-4F87-8BF2-9BC1510C5FCB}" uniqueName="4" name="c/n" queryTableFieldId="4" dataDxfId="7">
       <calculatedColumnFormula>InsertionSort10020[[#This Row],[c]]/InsertionSort10020[[#This Row],[n]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{6C0D5E71-22A3-45A2-AD02-E3E395CAB90A}" uniqueName="5" name="s/n" queryTableFieldId="5" dataDxfId="8">
+    <tableColumn id="5" xr3:uid="{6C0D5E71-22A3-45A2-AD02-E3E395CAB90A}" uniqueName="5" name="s/n" queryTableFieldId="5" dataDxfId="6">
       <calculatedColumnFormula>InsertionSort10020[[#This Row],[s]]/InsertionSort10020[[#This Row],[n]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -32360,7 +32360,7 @@
   <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z9" sqref="Z9"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>